<commit_message>
Update CoolTerm Capture 2021-01-21 14-12-19.xlsx
</commit_message>
<xml_diff>
--- a/Vent_Photon/dataReduction/CoolTerm Capture 2021-01-21 14-12-19.xlsx
+++ b/Vent_Photon/dataReduction/CoolTerm Capture 2021-01-21 14-12-19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10512" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10512" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Duct ST HS" sheetId="2" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Room Response" sheetId="4" r:id="rId3"/>
     <sheet name="Potential" sheetId="5" r:id="rId4"/>
     <sheet name="CoolTerm Capture 2021-01-21 14-" sheetId="1" r:id="rId5"/>
+    <sheet name="HalfStep Data" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="41">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -110,6 +111,42 @@
   </si>
   <si>
     <t>T_thermostat = 68 F</t>
+  </si>
+  <si>
+    <t>time_s</t>
+  </si>
+  <si>
+    <t>y1_dot</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>dT_fit_1</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>Tau_1=</t>
+  </si>
+  <si>
+    <t>dT_1</t>
+  </si>
+  <si>
+    <t>Tau_2=</t>
+  </si>
+  <si>
+    <t>dT_2=</t>
+  </si>
+  <si>
+    <t>dT_fit_2</t>
+  </si>
+  <si>
+    <t>y2_dot</t>
+  </si>
+  <si>
+    <t>y2</t>
   </si>
 </sst>
 </file>
@@ -601,10 +638,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -678,7 +718,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -832,11 +871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="526273856"/>
-        <c:axId val="526274248"/>
+        <c:axId val="526260112"/>
+        <c:axId val="526258152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="526273856"/>
+        <c:axId val="526260112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,12 +932,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526274248"/>
+        <c:crossAx val="526258152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526274248"/>
+        <c:axId val="526258152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526273856"/>
+        <c:crossAx val="526260112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1015,7 +1054,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1183,11 +1221,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="530110152"/>
-        <c:axId val="530110544"/>
+        <c:axId val="526256976"/>
+        <c:axId val="526252272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="530110152"/>
+        <c:axId val="526256976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,12 +1282,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530110544"/>
+        <c:crossAx val="526252272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="530110544"/>
+        <c:axId val="526252272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530110152"/>
+        <c:crossAx val="526256976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2810,11 +2848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="525120472"/>
-        <c:axId val="525123216"/>
+        <c:axId val="526250704"/>
+        <c:axId val="526260504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="525120472"/>
+        <c:axId val="526250704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -2873,12 +2911,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525123216"/>
+        <c:crossAx val="526260504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="525123216"/>
+        <c:axId val="526260504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -2937,7 +2975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525120472"/>
+        <c:crossAx val="526250704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4442,11 +4480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="537405024"/>
-        <c:axId val="537405808"/>
+        <c:axId val="526248744"/>
+        <c:axId val="526253056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="537405024"/>
+        <c:axId val="526248744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="14"/>
@@ -4504,12 +4542,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537405808"/>
+        <c:crossAx val="526253056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="537405808"/>
+        <c:axId val="526253056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4566,7 +4604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537405024"/>
+        <c:crossAx val="526248744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4793,11 +4831,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="529149608"/>
-        <c:axId val="529153528"/>
+        <c:axId val="526259720"/>
+        <c:axId val="526251488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="529149608"/>
+        <c:axId val="526259720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14.3"/>
@@ -4855,12 +4893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529153528"/>
+        <c:crossAx val="526251488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529153528"/>
+        <c:axId val="526251488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10"/>
@@ -4918,7 +4956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529149608"/>
+        <c:crossAx val="526259720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7811,11 +7849,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="529158232"/>
-        <c:axId val="529155096"/>
+        <c:axId val="526254232"/>
+        <c:axId val="526255408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="529158232"/>
+        <c:axId val="526254232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -7874,12 +7912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529155096"/>
+        <c:crossAx val="526255408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529155096"/>
+        <c:axId val="526255408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -7937,7 +7975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529158232"/>
+        <c:crossAx val="526254232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10873,11 +10911,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="529146080"/>
-        <c:axId val="529150392"/>
+        <c:axId val="526263248"/>
+        <c:axId val="526264032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="529146080"/>
+        <c:axId val="526263248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -10936,12 +10974,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529150392"/>
+        <c:crossAx val="526264032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529150392"/>
+        <c:axId val="526264032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="68"/>
@@ -11000,7 +11038,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529146080"/>
+        <c:crossAx val="526263248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11079,6 +11117,1461 @@
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HalfStep Data'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4530</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6060</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8460</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$F$2:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.7999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.7000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.1000000000000085</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.4000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.2000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.0999999999999943</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HalfStep Data'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dT_fit_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4530</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6060</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8460</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$G$2:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.682231969774307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.309163818525366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.078254003710743</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.134980614046608</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.310993925856287</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.7446767091966</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.355452957791648</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.087943646400227</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.904087364704147</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.777724913456055</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.6908773554715</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.631187959979535</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.590164078400392</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.561968804416658</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.529271990519781</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.513827109253693</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.506531463932539</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.503085245102167</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.500688411233742</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.500003612450616</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.500000179853327</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.500000000010484</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.500000000000011</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="530204216"/>
+        <c:axId val="530200688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="530204216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530200688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="530200688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530204216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HalfStep Data'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>diff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4530</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6060</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8460</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$H$2:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.9822319697743112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89083618147462929</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8217459962892484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1650193859533893</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3890060741437082</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7553232908034069</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0445470422083574</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4120563535997732</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3959126352958506</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3222750865439394</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2091226445284917</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7688120400204568</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2098359215996055</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3380311955833477</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8707280094802243</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6861728907463096</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.59346853606746919</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.39691475489783912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9311588766251901E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.9000036124506217</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.3000001798533241</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.7000000000104869</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-6.8000000000000078</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-6.3999999999999915</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-7.0999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-7.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-7.4000000000000057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HalfStep Data'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dT_fit_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4530</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6060</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8460</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HalfStep Data'!$I$2:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6296486804249888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.26844136751071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.572561270539393</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9106196463758671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5918553115381107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2809612961697274</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9777432813906559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6820117460710731</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3935818483745273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1122733102257683</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.837910304631083</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5703213457807017</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3093391818645834</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0548006905345897</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5644222743266001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0979598956895016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.6542471557072993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.23217454141039617</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.55122044312885699</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-2.7509337633326716</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.7024280470971469</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.756470711660473</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-6.5694625667667559</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-7.6472338121598646</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-7.9355554296387147</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-7.9921083480932591</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-7.9993838066716219</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-7.9999887140255126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="531750304"/>
+        <c:axId val="531754224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="531750304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531754224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="531754224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531750304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -11323,6 +12816,86 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -14974,6 +16547,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -15246,6 +17851,73 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16218,8 +18890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16566,7 +19238,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M3:M66" si="3">G6-H6</f>
+        <f t="shared" ref="M6:M66" si="3">G6-H6</f>
         <v>16.800000000000004</v>
       </c>
       <c r="N6">
@@ -16602,7 +19274,7 @@
         <v>29.999999999998295</v>
       </c>
       <c r="AG6">
-        <f t="shared" ref="AG6:AG15" si="6">1-(AD6-$AD$11)/($AD$5-$AD$11)</f>
+        <f t="shared" ref="AG6:AG11" si="6">1-(AD6-$AD$11)/($AD$5-$AD$11)</f>
         <v>0.66820276497695774</v>
       </c>
     </row>
@@ -28663,6 +31335,1537 @@
       </c>
       <c r="P225" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1">
+        <v>40</v>
+      </c>
+      <c r="R1">
+        <f>12/60+19/3600+14</f>
+        <v>14.205277777777777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3">
+        <v>83.3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43.8</v>
+      </c>
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>39.5</v>
+      </c>
+      <c r="G2">
+        <f>$F$2-$Q$2*(1-EXP(-B2/$Q$1))</f>
+        <v>39.5</v>
+      </c>
+      <c r="H2">
+        <f>F2-G2</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>7+$H$2-$Q$4*(1-EXP(-B2/$Q$3))</f>
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <f>G2</f>
+        <v>39.5</v>
+      </c>
+      <c r="M2">
+        <f>K2</f>
+        <v>39.5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="3">
+        <f>A3*60</f>
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3">
+        <v>83.3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>53.6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F30" si="0">D3-E3</f>
+        <v>29.699999999999996</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G30" si="1">$F$2-$Q$2*(1-EXP(-B3/$Q$1))</f>
+        <v>31.682231969774307</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H30" si="2">F3-G3</f>
+        <v>-1.9822319697743112</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I30" si="3">7+$H$2-$Q$4*(1-EXP(-B3/$Q$3))</f>
+        <v>6.6296486804249888</v>
+      </c>
+      <c r="J3">
+        <f>(F3-K2)/$Q$1</f>
+        <v>-0.24500000000000011</v>
+      </c>
+      <c r="K3">
+        <f>K2+(B3-B2)*J3</f>
+        <v>35.824999999999996</v>
+      </c>
+      <c r="L3">
+        <f>(K3-M2)/$Q$3</f>
+        <v>-6.1250000000000072E-3</v>
+      </c>
+      <c r="M3">
+        <f>M2+(B3-B2)*L3</f>
+        <v>39.408124999999998</v>
+      </c>
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B30" si="4">A4*60</f>
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3">
+        <v>83.3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>56.1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>27.199999999999996</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>26.309163818525366</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.89083618147462929</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>6.26844136751071</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J30" si="5">(F4-K3)/$Q$1</f>
+        <v>-0.21562500000000001</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K30" si="6">K3+(B4-B3)*J4</f>
+        <v>32.590624999999996</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L30" si="7">(K4-M3)/$Q$3</f>
+        <v>-1.1362500000000005E-2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M30" si="8">M3+(B4-B3)*L4</f>
+        <v>39.2376875</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="C5" s="3">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3">
+        <v>85.1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>60.2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>24.899999999999991</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>20.078254003710743</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>4.8217459962892484</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>5.572561270539393</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>-0.19226562500000011</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>26.822656249999994</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="7"/>
+        <v>-2.0691718750000008E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="8"/>
+        <v>38.616935937500003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="C6" s="3">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>85.1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>61.8</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>23.299999999999997</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>17.134980614046608</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>6.1650193859533893</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>4.9106196463758671</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>-8.8066406249999923E-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>24.180664062499996</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="7"/>
+        <v>-2.4060453125000009E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="8"/>
+        <v>37.895122343750003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="C7" s="3">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3">
+        <v>85.1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>62.4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>22.699999999999996</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>16.310993925856287</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>6.3890060741437082</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>4.5918553115381107</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>-3.7016601562500015E-2</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>23.625415039062496</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="7"/>
+        <v>-2.3782845507812511E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="8"/>
+        <v>37.538379661132815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="C8" s="3">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E8" s="3">
+        <v>62.4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>22.500000000000007</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>15.7446767091966</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>6.7553232908034069</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>4.2809612961697274</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>-2.8135375976562217E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>23.203384399414063</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>-2.3891658769531254E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>37.180004779589844</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="4"/>
+        <v>135</v>
+      </c>
+      <c r="C9" s="3">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>64.5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>20.400000000000006</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>15.355452957791648</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>5.0445470422083574</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>3.9777432813906559</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>-7.0084609985351418E-2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>22.152115249633791</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="7"/>
+        <v>-2.5046482549926755E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>36.80430754134094</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="C10" s="3">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>15.087943646400227</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>3.4120563535997732</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>3.6820117460710731</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>-9.1302881240844777E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>20.782572031021118</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>-2.6702892517199702E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
+        <v>36.403764153582941</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="C11" s="3">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>66.3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>17.299999999999997</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>14.904087364704147</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>2.3959126352958506</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>3.3935818483745273</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>-8.7064300775528028E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>19.476607519388196</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="7"/>
+        <v>-2.8211927723657909E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="8"/>
+        <v>35.980585237728071</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="C12" s="3">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E12" s="3">
+        <v>66.5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>17.099999999999994</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>14.777724913456055</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>2.3222750865439394</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>3.1122733102257683</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>-5.9415187984705041E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>18.585379699617619</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>-2.899200923018409E-2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="8"/>
+        <v>35.54570509927531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>3.25</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="C13" s="3">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E13" s="3">
+        <v>66.7</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>16.899999999999991</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>14.6908773554715</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>2.2091226445284917</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>2.837910304631083</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>-4.2134492490440677E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
+        <v>17.953362312261007</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="7"/>
+        <v>-2.9320571311690503E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="8"/>
+        <v>35.105896529599953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
+      <c r="C14" s="3">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E14" s="3">
+        <v>67.2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>16.399999999999991</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>14.631187959979535</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>1.7688120400204568</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>2.5703213457807017</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>-3.8834057806525379E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>17.370851445163126</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="7"/>
+        <v>-2.9558408474061378E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="8"/>
+        <v>34.662520402489029</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="4"/>
+        <v>225</v>
+      </c>
+      <c r="C15" s="3">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E15" s="3">
+        <v>67.8</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>15.799999999999997</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>14.590164078400392</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>1.2098359215996055</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>2.3093391818645834</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>-3.9271286129078223E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="6"/>
+        <v>16.781782153226953</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="7"/>
+        <v>-2.9801230415436794E-2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="8"/>
+        <v>34.215501946257476</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="C16" s="3">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>68</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>16.900000000000006</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>14.561968804416658</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>2.3380311955833477</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2.0548006905345897</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>2.9554461693263256E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>16.826113845766848</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="7"/>
+        <v>-2.8982313500817713E-2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="8"/>
+        <v>33.78076724374521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="C17" s="3">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E17" s="3">
+        <v>68.5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>16.400000000000006</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>14.529271990519781</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>1.8707280094802243</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>1.5644222743266001</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>-1.0652846144171058E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>16.506528461441718</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="7"/>
+        <v>-2.879039797050582E-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="8"/>
+        <v>32.917055304630033</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="C18" s="3">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3">
+        <v>85.2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>69</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>16.200000000000003</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>14.513827109253693</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>1.6861728907463096</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>1.0979598956895016</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>-7.6632115360428799E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>16.276632115360432</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="7"/>
+        <v>-2.7734038648782669E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="8"/>
+        <v>32.085034145166553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="4"/>
+        <v>330</v>
+      </c>
+      <c r="C19" s="3">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <v>85.2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>15.100000000000009</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>14.506531463932539</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>0.59346853606746919</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>0.6542471557072993</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>-2.9415802884010578E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>15.394158028840113</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="7"/>
+        <v>-2.7818126860544065E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="8"/>
+        <v>31.250490339350232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="C20" s="3">
+        <v>22</v>
+      </c>
+      <c r="D20" s="3">
+        <v>85.2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>70.3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>14.900000000000006</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>14.503085245102167</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>0.39691475489783912</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0.23217454141039617</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>-1.2353950721002694E-2</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>15.023539507210032</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
+        <v>-2.7044918053567003E-2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="8"/>
+        <v>30.439142797743223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="4"/>
+        <v>420</v>
+      </c>
+      <c r="C21" s="3">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3">
+        <v>85.6</v>
+      </c>
+      <c r="E21" s="3">
+        <v>71</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>14.599999999999994</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>14.500688411233742</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>9.9311588766251901E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>-0.55122044312885699</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>-1.0588487680250936E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>14.388230246394976</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="7"/>
+        <v>-2.6751520918913745E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="8"/>
+        <v>28.8340515426084</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="4"/>
+        <v>630</v>
+      </c>
+      <c r="C22" s="3">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="E22" s="3">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>10.599999999999994</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>14.500003612450616</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>-3.9000036124506217</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>-2.7509337633326716</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>-9.4705756159874532E-2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>-5.499978547178678</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>-5.7223383482978465E-2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="8"/>
+        <v>16.817141011182922</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="4"/>
+        <v>750</v>
+      </c>
+      <c r="C23" s="3">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3">
+        <v>84.4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>73.2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>11.200000000000003</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>14.500000179853327</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>-3.3000001798533241</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>-3.7024280470971469</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>0.417499463679467</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>44.599957094357364</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>4.6304693471957405E-2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="8"/>
+        <v>22.373704227817811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="4"/>
+        <v>1140</v>
+      </c>
+      <c r="C24" s="3">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3">
+        <v>83.8</v>
+      </c>
+      <c r="E24" s="3">
+        <v>75</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>8.7999999999999972</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>14.500000000010484</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>-5.7000000000104869</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>-5.756470711660473</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>-0.89499892735893416</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>-304.44962457562696</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>-0.54470554800574134</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="8"/>
+        <v>-190.06145949442129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="4"/>
+        <v>1410</v>
+      </c>
+      <c r="C25" s="3">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3">
+        <v>83.4</v>
+      </c>
+      <c r="E25" s="3">
+        <v>75.7</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>7.7000000000000028</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>14.500000000000011</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>-6.8000000000000078</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>-6.5694625667667559</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>7.8037406143906738</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>1802.5603413098549</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>3.3210363346737939</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>706.61835086750307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>37.5</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="4"/>
+        <v>2250</v>
+      </c>
+      <c r="C26" s="3">
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E26" s="3">
+        <v>76.8</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000085</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>-6.3999999999999915</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>-7.6472338121598646</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>-44.861508532746377</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>-35881.106826197101</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>-60.979541961774338</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>-50516.196897022943</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>54.5</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="4"/>
+        <v>3270</v>
+      </c>
+      <c r="C27" s="3">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="E27" s="3">
+        <v>77.5</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>7.4000000000000057</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>-7.0999999999999943</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>-7.9355554296387147</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>897.21267065492759</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>879275.81724182901</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>1549.6533568980865</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="8"/>
+        <v>1530130.2271390252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>75.5</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="4"/>
+        <v>4530</v>
+      </c>
+      <c r="C28" s="3">
+        <v>22</v>
+      </c>
+      <c r="D28" s="3">
+        <v>86.9</v>
+      </c>
+      <c r="E28" s="3">
+        <v>79.7</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000028</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>-7.2999999999999972</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>-7.9921083480932591</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>-21981.715431045726</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>-26817685.625875786</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>-47246.359755024685</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>-58000283.064192079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>101</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="4"/>
+        <v>6060</v>
+      </c>
+      <c r="C29" s="3">
+        <v>22</v>
+      </c>
+      <c r="D29" s="3">
+        <v>89</v>
+      </c>
+      <c r="E29" s="3">
+        <v>82.5</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>-7.9993838066716219</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>670442.30314689467</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>998959038.18887305</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="7"/>
+        <v>1761598.8687551084</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="8"/>
+        <v>2637245986.1311235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>141</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="4"/>
+        <v>8460</v>
+      </c>
+      <c r="C30" s="3">
+        <v>22</v>
+      </c>
+      <c r="D30" s="3">
+        <v>87.8</v>
+      </c>
+      <c r="E30" s="3">
+        <v>80.7</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>7.0999999999999943</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>-7.4000000000000057</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>-7.9999887140255126</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>-24973975.777221825</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>-58938582827.143509</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="7"/>
+        <v>-102626381.35545772</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>-243666069266.96741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>